<commit_message>
minor update to abbrs list
</commit_message>
<xml_diff>
--- a/abbrs.xlsx
+++ b/abbrs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="630" windowWidth="28800" windowHeight="12090"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="28800" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -323,9 +323,6 @@
     <t>f/</t>
   </si>
   <si>
-    <t>for</t>
-  </si>
-  <si>
     <t>fcst</t>
   </si>
   <si>
@@ -1815,6 +1812,9 @@
   </si>
   <si>
     <t>pgm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for </t>
   </si>
 </sst>
 </file>
@@ -2171,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="A201" sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2221,10 +2221,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,7 +2400,7 @@
         <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2411,7 +2411,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>1</v>
@@ -2584,10 +2584,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2595,10 +2595,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2675,7 +2675,7 @@
         <v>72</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2686,7 +2686,7 @@
         <v>72</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2749,10 +2749,10 @@
         <v>1</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2760,10 +2760,10 @@
         <v>1</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2771,10 +2771,10 @@
         <v>1</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2782,10 +2782,10 @@
         <v>1</v>
       </c>
       <c r="B55" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2793,10 +2793,10 @@
         <v>1</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2804,10 +2804,10 @@
         <v>1</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2815,10 +2815,10 @@
         <v>1</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2826,10 +2826,10 @@
         <v>1</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2837,10 +2837,10 @@
         <v>1</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2848,10 +2848,10 @@
         <v>1</v>
       </c>
       <c r="B61" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2859,10 +2859,10 @@
         <v>1</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2870,10 +2870,10 @@
         <v>1</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2881,10 +2881,10 @@
         <v>1</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2892,10 +2892,10 @@
         <v>1</v>
       </c>
       <c r="B65" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>568</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2903,10 +2903,10 @@
         <v>1</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2914,10 +2914,10 @@
         <v>1</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2925,10 +2925,10 @@
         <v>1</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2936,10 +2936,10 @@
         <v>1</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2947,10 +2947,10 @@
         <v>1</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2958,10 +2958,10 @@
         <v>1</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2969,10 +2969,10 @@
         <v>1</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2980,10 +2980,10 @@
         <v>1</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2991,10 +2991,10 @@
         <v>1</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3002,10 +3002,10 @@
         <v>1</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3013,10 +3013,10 @@
         <v>1</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3024,10 +3024,10 @@
         <v>1</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3035,10 +3035,10 @@
         <v>1</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3046,10 +3046,10 @@
         <v>1</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3057,10 +3057,10 @@
         <v>1</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -3068,10 +3068,10 @@
         <v>1</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -3079,10 +3079,10 @@
         <v>1</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -3090,10 +3090,10 @@
         <v>1</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -3101,10 +3101,10 @@
         <v>1</v>
       </c>
       <c r="B84" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>570</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3112,10 +3112,10 @@
         <v>1</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3123,10 +3123,10 @@
         <v>1</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3134,10 +3134,10 @@
         <v>1</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3145,10 +3145,10 @@
         <v>1</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3156,10 +3156,10 @@
         <v>1</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3167,10 +3167,10 @@
         <v>1</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3178,10 +3178,10 @@
         <v>1</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3189,10 +3189,10 @@
         <v>1</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3200,10 +3200,10 @@
         <v>1</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3211,10 +3211,10 @@
         <v>1</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3222,10 +3222,10 @@
         <v>1</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3233,10 +3233,10 @@
         <v>1</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3244,10 +3244,10 @@
         <v>1</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3255,10 +3255,10 @@
         <v>1</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3266,10 +3266,10 @@
         <v>1</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3277,7 +3277,7 @@
         <v>1</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>83</v>
@@ -3288,10 +3288,10 @@
         <v>1</v>
       </c>
       <c r="B101" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>557</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3376,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>99</v>
+        <v>596</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>98</v>
@@ -3387,10 +3387,10 @@
         <v>1</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3398,10 +3398,10 @@
         <v>1</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3409,10 +3409,10 @@
         <v>1</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3420,10 +3420,10 @@
         <v>1</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3431,10 +3431,10 @@
         <v>1</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3442,10 +3442,10 @@
         <v>1</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3453,10 +3453,10 @@
         <v>1</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3464,10 +3464,10 @@
         <v>1</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3475,10 +3475,10 @@
         <v>1</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3486,10 +3486,10 @@
         <v>1</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -3497,10 +3497,10 @@
         <v>1</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3508,10 +3508,10 @@
         <v>1</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3519,10 +3519,10 @@
         <v>1</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -3530,10 +3530,10 @@
         <v>1</v>
       </c>
       <c r="B123" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>562</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3541,10 +3541,10 @@
         <v>1</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3552,10 +3552,10 @@
         <v>1</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3563,10 +3563,10 @@
         <v>1</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3574,10 +3574,10 @@
         <v>1</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3585,10 +3585,10 @@
         <v>1</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -3596,10 +3596,10 @@
         <v>1</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3607,10 +3607,10 @@
         <v>1</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -3618,10 +3618,10 @@
         <v>1</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -3629,10 +3629,10 @@
         <v>1</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -3640,10 +3640,10 @@
         <v>1</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -3651,10 +3651,10 @@
         <v>1</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -3662,10 +3662,10 @@
         <v>1</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -3673,10 +3673,10 @@
         <v>1</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -3684,10 +3684,10 @@
         <v>1</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -3695,10 +3695,10 @@
         <v>1</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -3706,10 +3706,10 @@
         <v>1</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -3717,10 +3717,10 @@
         <v>1</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -3728,10 +3728,10 @@
         <v>1</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -3739,10 +3739,10 @@
         <v>1</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -3750,10 +3750,10 @@
         <v>1</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -3761,10 +3761,10 @@
         <v>1</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -3772,10 +3772,10 @@
         <v>1</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -3783,10 +3783,10 @@
         <v>1</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3794,10 +3794,10 @@
         <v>1</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3805,10 +3805,10 @@
         <v>1</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3816,10 +3816,10 @@
         <v>1</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3827,10 +3827,10 @@
         <v>1</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3838,10 +3838,10 @@
         <v>1</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3849,10 +3849,10 @@
         <v>1</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3860,10 +3860,10 @@
         <v>1</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -3871,10 +3871,10 @@
         <v>1</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -3882,10 +3882,10 @@
         <v>1</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -3893,10 +3893,10 @@
         <v>1</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3904,10 +3904,10 @@
         <v>1</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -3915,10 +3915,10 @@
         <v>1</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -3926,10 +3926,10 @@
         <v>1</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -3937,10 +3937,10 @@
         <v>1</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -3948,10 +3948,10 @@
         <v>1</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -3959,10 +3959,10 @@
         <v>1</v>
       </c>
       <c r="B162" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="C162" s="3" t="s">
         <v>580</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -3970,10 +3970,10 @@
         <v>1</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -3981,10 +3981,10 @@
         <v>1</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -3992,10 +3992,10 @@
         <v>1</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -4003,10 +4003,10 @@
         <v>1</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -4014,7 +4014,7 @@
         <v>1</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>2</v>
@@ -4025,10 +4025,10 @@
         <v>1</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -4036,10 +4036,10 @@
         <v>1</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,10 +4047,10 @@
         <v>1</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -4058,10 +4058,10 @@
         <v>1</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -4069,10 +4069,10 @@
         <v>1</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -4080,10 +4080,10 @@
         <v>1</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -4091,10 +4091,10 @@
         <v>1</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -4102,10 +4102,10 @@
         <v>1</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -4113,10 +4113,10 @@
         <v>1</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -4124,10 +4124,10 @@
         <v>1</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -4135,10 +4135,10 @@
         <v>1</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -4146,10 +4146,10 @@
         <v>1</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -4157,10 +4157,10 @@
         <v>1</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -4168,10 +4168,10 @@
         <v>1</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -4179,10 +4179,10 @@
         <v>1</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -4190,10 +4190,10 @@
         <v>1</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -4201,10 +4201,10 @@
         <v>1</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -4212,10 +4212,10 @@
         <v>1</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -4223,10 +4223,10 @@
         <v>1</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -4234,10 +4234,10 @@
         <v>1</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -4245,10 +4245,10 @@
         <v>1</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -4256,10 +4256,10 @@
         <v>1</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -4267,10 +4267,10 @@
         <v>1</v>
       </c>
       <c r="B190" s="6" t="s">
+        <v>586</v>
+      </c>
+      <c r="C190" s="3" t="s">
         <v>587</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -4278,10 +4278,10 @@
         <v>1</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -4289,10 +4289,10 @@
         <v>1</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -4300,10 +4300,10 @@
         <v>1</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -4311,10 +4311,10 @@
         <v>1</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -4322,10 +4322,10 @@
         <v>1</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -4333,10 +4333,10 @@
         <v>1</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -4344,10 +4344,10 @@
         <v>1</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -4355,10 +4355,10 @@
         <v>1</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -4366,10 +4366,10 @@
         <v>1</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -4377,10 +4377,10 @@
         <v>1</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -4388,10 +4388,10 @@
         <v>1</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -4399,10 +4399,10 @@
         <v>1</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -4410,10 +4410,10 @@
         <v>1</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -4421,10 +4421,10 @@
         <v>1</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -4432,10 +4432,10 @@
         <v>1</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -4443,10 +4443,10 @@
         <v>1</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -4454,10 +4454,10 @@
         <v>1</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -4465,10 +4465,10 @@
         <v>1</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -4476,10 +4476,10 @@
         <v>1</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -4487,10 +4487,10 @@
         <v>1</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -4498,10 +4498,10 @@
         <v>1</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -4509,10 +4509,10 @@
         <v>1</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -4520,10 +4520,10 @@
         <v>1</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -4531,10 +4531,10 @@
         <v>1</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -4542,10 +4542,10 @@
         <v>1</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -4553,10 +4553,10 @@
         <v>1</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -4564,10 +4564,10 @@
         <v>1</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -4575,10 +4575,10 @@
         <v>1</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -4586,10 +4586,10 @@
         <v>1</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -4597,10 +4597,10 @@
         <v>1</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -4608,10 +4608,10 @@
         <v>1</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -4619,10 +4619,10 @@
         <v>1</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -4630,10 +4630,10 @@
         <v>1</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -4641,10 +4641,10 @@
         <v>1</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -4652,10 +4652,10 @@
         <v>1</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -4663,10 +4663,10 @@
         <v>1</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -4674,10 +4674,10 @@
         <v>1</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -4685,10 +4685,10 @@
         <v>1</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -4696,10 +4696,10 @@
         <v>1</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -4707,10 +4707,10 @@
         <v>1</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -4718,10 +4718,10 @@
         <v>1</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -4729,10 +4729,10 @@
         <v>1</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -4740,10 +4740,10 @@
         <v>1</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -4751,10 +4751,10 @@
         <v>1</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -4762,10 +4762,10 @@
         <v>1</v>
       </c>
       <c r="B235" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -4773,10 +4773,10 @@
         <v>1</v>
       </c>
       <c r="B236" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -4784,10 +4784,10 @@
         <v>1</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -4795,10 +4795,10 @@
         <v>1</v>
       </c>
       <c r="B238" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -4806,10 +4806,10 @@
         <v>1</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -4817,10 +4817,10 @@
         <v>1</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -4828,10 +4828,10 @@
         <v>1</v>
       </c>
       <c r="B241" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C241" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -4839,10 +4839,10 @@
         <v>1</v>
       </c>
       <c r="B242" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="C242" s="3" t="s">
         <v>540</v>
-      </c>
-      <c r="C242" s="3" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -4850,10 +4850,10 @@
         <v>1</v>
       </c>
       <c r="B243" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -4861,10 +4861,10 @@
         <v>1</v>
       </c>
       <c r="B244" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C244" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -4872,10 +4872,10 @@
         <v>1</v>
       </c>
       <c r="B245" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -4883,10 +4883,10 @@
         <v>1</v>
       </c>
       <c r="B246" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -4894,10 +4894,10 @@
         <v>1</v>
       </c>
       <c r="B247" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -4905,10 +4905,10 @@
         <v>1</v>
       </c>
       <c r="B248" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -4916,10 +4916,10 @@
         <v>1</v>
       </c>
       <c r="B249" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -4927,10 +4927,10 @@
         <v>1</v>
       </c>
       <c r="B250" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -4938,10 +4938,10 @@
         <v>1</v>
       </c>
       <c r="B251" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -4949,10 +4949,10 @@
         <v>1</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -4960,10 +4960,10 @@
         <v>1</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -4971,10 +4971,10 @@
         <v>1</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -4982,10 +4982,10 @@
         <v>1</v>
       </c>
       <c r="B255" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C255" s="3" t="s">
         <v>455</v>
-      </c>
-      <c r="C255" s="3" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -4993,10 +4993,10 @@
         <v>1</v>
       </c>
       <c r="B256" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -5004,10 +5004,10 @@
         <v>1</v>
       </c>
       <c r="B257" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -5015,10 +5015,10 @@
         <v>1</v>
       </c>
       <c r="B258" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -5026,10 +5026,10 @@
         <v>1</v>
       </c>
       <c r="B259" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -5037,10 +5037,10 @@
         <v>1</v>
       </c>
       <c r="B260" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -5048,10 +5048,10 @@
         <v>1</v>
       </c>
       <c r="B261" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -5059,10 +5059,10 @@
         <v>1</v>
       </c>
       <c r="B262" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -5070,10 +5070,10 @@
         <v>1</v>
       </c>
       <c r="B263" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -5081,10 +5081,10 @@
         <v>1</v>
       </c>
       <c r="B264" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -5092,10 +5092,10 @@
         <v>1</v>
       </c>
       <c r="B265" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -5103,10 +5103,10 @@
         <v>1</v>
       </c>
       <c r="B266" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -5114,10 +5114,10 @@
         <v>1</v>
       </c>
       <c r="B267" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="C267" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="C267" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -5125,10 +5125,10 @@
         <v>1</v>
       </c>
       <c r="B268" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -5136,10 +5136,10 @@
         <v>1</v>
       </c>
       <c r="B269" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -5147,10 +5147,10 @@
         <v>1</v>
       </c>
       <c r="B270" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -5158,10 +5158,10 @@
         <v>1</v>
       </c>
       <c r="B271" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -5169,10 +5169,10 @@
         <v>1</v>
       </c>
       <c r="B272" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -5180,10 +5180,10 @@
         <v>1</v>
       </c>
       <c r="B273" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -5191,10 +5191,10 @@
         <v>1</v>
       </c>
       <c r="B274" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -5202,10 +5202,10 @@
         <v>1</v>
       </c>
       <c r="B275" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C275" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -5213,10 +5213,10 @@
         <v>1</v>
       </c>
       <c r="B276" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C276" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -5224,10 +5224,10 @@
         <v>1</v>
       </c>
       <c r="B277" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -5235,10 +5235,10 @@
         <v>1</v>
       </c>
       <c r="B278" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -5246,10 +5246,10 @@
         <v>1</v>
       </c>
       <c r="B279" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C279" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -5257,10 +5257,10 @@
         <v>1</v>
       </c>
       <c r="B280" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -5268,10 +5268,10 @@
         <v>1</v>
       </c>
       <c r="B281" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C281" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -5279,10 +5279,10 @@
         <v>1</v>
       </c>
       <c r="B282" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C282" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -5290,10 +5290,10 @@
         <v>1</v>
       </c>
       <c r="B283" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -5301,10 +5301,10 @@
         <v>1</v>
       </c>
       <c r="B284" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -5312,10 +5312,10 @@
         <v>1</v>
       </c>
       <c r="B285" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -5323,10 +5323,10 @@
         <v>1</v>
       </c>
       <c r="B286" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C286" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -5334,10 +5334,10 @@
         <v>1</v>
       </c>
       <c r="B287" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -5345,10 +5345,10 @@
         <v>1</v>
       </c>
       <c r="B288" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C288" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -5356,10 +5356,10 @@
         <v>1</v>
       </c>
       <c r="B289" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C289" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -5367,10 +5367,10 @@
         <v>1</v>
       </c>
       <c r="B290" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C290" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -5378,10 +5378,10 @@
         <v>1</v>
       </c>
       <c r="B291" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -5389,10 +5389,10 @@
         <v>1</v>
       </c>
       <c r="B292" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -5400,10 +5400,10 @@
         <v>1</v>
       </c>
       <c r="B293" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -5411,10 +5411,10 @@
         <v>1</v>
       </c>
       <c r="B294" s="6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C294" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -5422,10 +5422,10 @@
         <v>1</v>
       </c>
       <c r="B295" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -5433,10 +5433,10 @@
         <v>1</v>
       </c>
       <c r="B296" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C296" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -5444,10 +5444,10 @@
         <v>1</v>
       </c>
       <c r="B297" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -5455,10 +5455,10 @@
         <v>1</v>
       </c>
       <c r="B298" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C298" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -5466,10 +5466,10 @@
         <v>1</v>
       </c>
       <c r="B299" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C299" s="3" t="s">
         <v>543</v>
-      </c>
-      <c r="C299" s="3" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -5477,10 +5477,10 @@
         <v>1</v>
       </c>
       <c r="B300" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="C300" s="3" t="s">
         <v>545</v>
-      </c>
-      <c r="C300" s="3" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -5488,10 +5488,10 @@
         <v>1</v>
       </c>
       <c r="B301" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C301" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -5499,10 +5499,10 @@
         <v>1</v>
       </c>
       <c r="B302" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -5510,10 +5510,10 @@
         <v>1</v>
       </c>
       <c r="B303" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -5521,10 +5521,10 @@
         <v>1</v>
       </c>
       <c r="B304" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C304" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -5532,10 +5532,10 @@
         <v>1</v>
       </c>
       <c r="B305" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C305" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -5543,10 +5543,10 @@
         <v>1</v>
       </c>
       <c r="B306" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C306" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -5554,10 +5554,10 @@
         <v>1</v>
       </c>
       <c r="B307" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C307" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -5565,10 +5565,10 @@
         <v>1</v>
       </c>
       <c r="B308" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C308" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -5576,10 +5576,10 @@
         <v>1</v>
       </c>
       <c r="B309" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C309" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -5587,10 +5587,10 @@
         <v>1</v>
       </c>
       <c r="B310" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C310" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -5598,10 +5598,10 @@
         <v>1</v>
       </c>
       <c r="B311" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C311" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -5609,10 +5609,10 @@
         <v>1</v>
       </c>
       <c r="B312" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C312" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added space detection functionality. does not work if it's the last word in the bullet and the space is at the end. also added import xlsx functionality
</commit_message>
<xml_diff>
--- a/abbrs.xlsx
+++ b/abbrs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="28800" windowHeight="12090"/>
+    <workbookView xWindow="0" yWindow="1680" windowWidth="28800" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2171,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>